<commit_message>
with folder re arrangement
</commit_message>
<xml_diff>
--- a/resources/data.xlsx
+++ b/resources/data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="19">
   <si>
     <t>EmpID</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Doli</t>
   </si>
   <si>
-    <t>shwenky</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
@@ -82,7 +79,7 @@
     <t xml:space="preserve">KafkaTest </t>
   </si>
   <si>
-    <t>01/01/2023</t>
+    <t>01/02/2023</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -496,15 +493,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
@@ -512,7 +509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="0">
         <v>1</v>
       </c>
@@ -520,15 +517,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="0">
         <v>2</v>
       </c>
       <c r="B3" t="s" s="0">
         <v>3</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -541,7 +535,7 @@
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,39 +548,39 @@
   <sheetData>
     <row r="1" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="C2" s="5">
         <v>1558</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="10">
-        <v>6988078</v>
+        <v>6988079</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1634,24 +1628,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C1" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" t="s" s="0">
         <v>14</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>